<commit_message>
Bump to 0.5.0-SNAPSHOT.  Uses caches for CellStyles and Fonts for use by the style tag.  Move WorkbookContext to the model package.  Started Cache unit tests.  Worked around POI bug that flips black and white font colors when the color is based on a theme.
</commit_message>
<xml_diff>
--- a/jett-core/templates/StyleTagTemplate.xlsx
+++ b/jett-core/templates/StyleTagTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="20115" windowHeight="11565" firstSheet="8" activeTab="12"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="20115" windowHeight="11565"/>
   </bookViews>
   <sheets>
     <sheet name="alignment" sheetId="1" r:id="rId1"/>
@@ -463,7 +463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -552,7 +552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -623,9 +623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -677,7 +675,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>